<commit_message>
adding nodejs files and new csvs
</commit_message>
<xml_diff>
--- a/csv/gadeaths.xlsx
+++ b/csv/gadeaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margot/Sites/GACOVID19/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A0E4DE-9025-9941-9396-29BF1E6D8722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75535D3-26F4-5747-AB1B-AA15686A1686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="25600" windowHeight="14900" xr2:uid="{13D2A8DC-F671-9B4B-9376-AD455D5769C0}"/>
+    <workbookView xWindow="-27460" yWindow="1100" windowWidth="25600" windowHeight="14900" xr2:uid="{13D2A8DC-F671-9B4B-9376-AD455D5769C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,244 +400,244 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection sqref="A1:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="D2" s="1">
         <v>43902</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="D3" s="1">
         <v>43908</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="C4">
         <v>10</v>
       </c>
-      <c r="B4" s="1">
+      <c r="D4" s="1">
         <v>43909</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="C5">
         <v>14</v>
       </c>
-      <c r="B5" s="1">
+      <c r="D5" s="1">
         <v>43910</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="C6">
         <v>20</v>
       </c>
-      <c r="B6" s="1">
+      <c r="D6" s="1">
         <v>43911</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="C7">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
+      <c r="D7" s="1">
         <v>43912</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="C8">
         <v>26</v>
       </c>
-      <c r="B8" s="1">
+      <c r="D8" s="1">
         <v>43913</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="B9">
+        <v>361</v>
+      </c>
+      <c r="C9">
         <v>38</v>
       </c>
-      <c r="B9" s="1">
+      <c r="D9" s="1">
         <v>43914</v>
       </c>
-      <c r="C9">
-        <v>361</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="B10">
+        <v>394</v>
+      </c>
+      <c r="C10">
         <v>40</v>
       </c>
-      <c r="B10" s="1">
+      <c r="D10" s="1">
         <v>43915</v>
       </c>
-      <c r="C10">
-        <v>394</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="B11">
+        <v>438</v>
+      </c>
+      <c r="C11">
         <v>47</v>
       </c>
-      <c r="B11" s="1">
+      <c r="D11" s="1">
         <v>43915</v>
       </c>
-      <c r="C11">
-        <v>438</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="B12">
+        <v>473</v>
+      </c>
+      <c r="C12">
         <v>48</v>
       </c>
-      <c r="B12" s="1">
+      <c r="D12" s="1">
         <v>43916</v>
       </c>
-      <c r="C12">
-        <v>473</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="B13">
+        <v>509</v>
+      </c>
+      <c r="C13">
         <v>56</v>
       </c>
-      <c r="B13" s="1">
+      <c r="D13" s="1">
         <v>43916</v>
       </c>
-      <c r="C13">
-        <v>509</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="B14">
+        <v>566</v>
+      </c>
+      <c r="C14">
         <v>64</v>
       </c>
-      <c r="B14" s="1">
+      <c r="D14" s="1">
         <v>43917</v>
       </c>
-      <c r="C14">
-        <v>566</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="B15">
+        <v>607</v>
+      </c>
+      <c r="C15">
         <v>65</v>
       </c>
-      <c r="B15" s="1">
+      <c r="D15" s="1">
         <v>43917</v>
       </c>
-      <c r="C15">
-        <v>607</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="B16">
+        <v>617</v>
+      </c>
+      <c r="C16">
         <v>69</v>
       </c>
-      <c r="B16" s="1">
+      <c r="D16" s="1">
         <v>43918</v>
       </c>
-      <c r="C16">
-        <v>617</v>
-      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="B17">
+        <v>660</v>
+      </c>
+      <c r="C17">
         <v>79</v>
       </c>
-      <c r="B17" s="1">
+      <c r="D17" s="1">
         <v>43918</v>
       </c>
-      <c r="C17">
-        <v>660</v>
-      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="1">
+      <c r="D18" s="1">
         <v>43919</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="B19">
+        <v>678</v>
+      </c>
+      <c r="C19">
         <v>83</v>
       </c>
-      <c r="B19" s="1">
+      <c r="D19" s="1">
         <v>43919</v>
       </c>
-      <c r="C19">
-        <v>678</v>
-      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="B20">
+        <v>707</v>
+      </c>
+      <c r="C20">
         <v>87</v>
       </c>
-      <c r="B20" s="1">
+      <c r="D20" s="1">
         <v>43920</v>
       </c>
-      <c r="C20">
-        <v>707</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="B21">
+        <v>771</v>
+      </c>
+      <c r="C21">
         <v>100</v>
       </c>
-      <c r="B21" s="1">
+      <c r="D21" s="1">
         <v>43920</v>
-      </c>
-      <c r="C21">
-        <v>771</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
+        <v>3817</v>
+      </c>
+      <c r="B22">
+        <v>818</v>
+      </c>
+      <c r="C22">
         <v>108</v>
       </c>
-      <c r="B22" s="1">
+      <c r="D22" s="1">
         <v>43921</v>
-      </c>
-      <c r="C22">
-        <v>818</v>
-      </c>
-      <c r="D22">
-        <v>3817</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>4117</v>
+      </c>
+      <c r="B23">
+        <v>885</v>
+      </c>
+      <c r="C23">
         <v>125</v>
       </c>
-      <c r="B23" s="1">
+      <c r="D23" s="1">
         <v>43921</v>
-      </c>
-      <c r="C23">
-        <v>885</v>
-      </c>
-      <c r="D23">
-        <v>4117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>